<commit_message>
Table 1 marine updated
</commit_message>
<xml_diff>
--- a/Table1_Marine.xlsx
+++ b/Table1_Marine.xlsx
@@ -12,36 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">Area_Sq_Km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion</t>
+  </si>
   <si>
     <t xml:space="preserve">Class</t>
   </si>
   <si>
-    <t xml:space="preserve">Area_Sq_Km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proportion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Area_Exclusive</t>
   </si>
   <si>
     <t xml:space="preserve">Area_Overlapped</t>
   </si>
   <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nautra_2000</t>
   </si>
   <si>
     <t xml:space="preserve">Fredninger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Habitatomrade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Habitatnaturtype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramsar</t>
   </si>
   <si>
     <t xml:space="preserve">Havstrategi_standard</t>
@@ -400,139 +394,105 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="n">
+        <v>30238.8931</v>
+      </c>
+      <c r="B2" t="n">
+        <v>28.7932954632323</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>30478.8135</v>
-      </c>
-      <c r="C2" t="n">
-        <v>29.0217462514941</v>
-      </c>
       <c r="D2" t="n">
-        <v>7332.2813</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>23146.5322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="n">
+        <v>26284.8191</v>
+      </c>
+      <c r="B3" t="n">
+        <v>25.0282495473987</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>21292.4538</v>
-      </c>
-      <c r="C3" t="n">
-        <v>20.2745487863319</v>
-      </c>
       <c r="D3" t="n">
-        <v>310.0434</v>
+        <v>7274.0322</v>
       </c>
       <c r="E3" t="n">
-        <v>20982.4104</v>
+        <v>19010.7869</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="n">
+        <v>19305.923</v>
+      </c>
+      <c r="B4" t="n">
+        <v>18.3829858881115</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="n">
-        <v>19979.9759</v>
-      </c>
-      <c r="C4" t="n">
-        <v>19.0248150795229</v>
-      </c>
       <c r="D4" t="n">
-        <v>0.0008</v>
+        <v>203.7476</v>
       </c>
       <c r="E4" t="n">
-        <v>19979.9751</v>
+        <v>19102.1754</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="n">
+        <v>7157.3432</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6.81517993426012</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="n">
-        <v>7589.0614</v>
-      </c>
-      <c r="C5" t="n">
-        <v>7.22625945520511</v>
-      </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2264.7899</v>
       </c>
       <c r="E5" t="n">
-        <v>7589.0614</v>
+        <v>4892.5533</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="n">
+        <v>4300.9158</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4.09530662985426</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="n">
-        <v>7279.4095</v>
-      </c>
-      <c r="C6" t="n">
-        <v>6.93141074437544</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>7279.4095</v>
+        <v>4300.9158</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="n">
+        <v>2378.0018</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2.26431927296632</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="n">
-        <v>7157.3432</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6.81517993426012</v>
-      </c>
       <c r="D7" t="n">
-        <v>2264.053</v>
+        <v>3.3514</v>
       </c>
       <c r="E7" t="n">
-        <v>4893.2902</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="n">
-        <v>4300.9158</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.09530662985426</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4300.9158</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="n">
-        <v>3415.9911</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3.25268655558269</v>
-      </c>
-      <c r="D9" t="n">
-        <v>8.3385</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3407.6526</v>
+        <v>2374.6504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>